<commit_message>
regression testing by using api
</commit_message>
<xml_diff>
--- a/TestSuite-API/reports/daily_reading_report.xlsx
+++ b/TestSuite-API/reports/daily_reading_report.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="report" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="report" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="106">
   <si>
     <t>Date
 Period</t>
@@ -265,6 +265,84 @@
   </si>
   <si>
     <t>['7ff9010202000057', '7ff9010202000069', '7ff9010202000131', '7ff9010202000163']</t>
+  </si>
+  <si>
+    <t>17-10-10 ~ 17-10-11</t>
+  </si>
+  <si>
+    <t>['7ff9010202000031', '7ff9010202000057', '7ff9010202000060', '7ff9010202000104', '7ff9010202000126']</t>
+  </si>
+  <si>
+    <t>17-10-11 ~ 17-10-12</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>97.56%</t>
+  </si>
+  <si>
+    <t>['7ff9010202000151', '7ff9010202000163']</t>
+  </si>
+  <si>
+    <t>17-10-12 ~ 17-10-13</t>
+  </si>
+  <si>
+    <t>['7ff9010202000059', '7ff9010202000082', '7ff9010202000097', '7ff9010202000106', '7ff9010202000123']</t>
+  </si>
+  <si>
+    <t>17-10-13 ~ 17-10-14</t>
+  </si>
+  <si>
+    <t>['7ff9010202000067', '7ff9010202000082', '7ff9010202000088', '7ff9010202000129', '7ff9010202000163']</t>
+  </si>
+  <si>
+    <t>17-10-14 ~ 17-10-15</t>
+  </si>
+  <si>
+    <t>['7ff9010202000057', '7ff9010202000121', '7ff9010202000146']</t>
+  </si>
+  <si>
+    <t>17-10-15 ~ 17-10-16</t>
+  </si>
+  <si>
+    <t>17-10-16 ~ 17-10-17</t>
+  </si>
+  <si>
+    <t>17-10-17 ~ 17-10-18</t>
+  </si>
+  <si>
+    <t>17-10-18 ~ 17-10-19</t>
+  </si>
+  <si>
+    <t>17-10-19 ~ 17-10-20</t>
+  </si>
+  <si>
+    <t>17-10-20 ~ 17-10-21</t>
+  </si>
+  <si>
+    <t>17-10-21 ~ 17-10-22</t>
+  </si>
+  <si>
+    <t>17-10-22 ~ 17-10-23</t>
+  </si>
+  <si>
+    <t>17-10-23 ~ 17-10-24</t>
+  </si>
+  <si>
+    <t>17-10-24 ~ 17-10-25</t>
+  </si>
+  <si>
+    <t>17-10-25 ~ 17-10-26</t>
+  </si>
+  <si>
+    <t>17-10-26 ~ 17-10-27</t>
+  </si>
+  <si>
+    <t>17-10-27 ~ 17-10-28</t>
   </si>
 </sst>
 </file>
@@ -646,10 +724,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -1363,6 +1441,798 @@
         <v>79</v>
       </c>
     </row>
+    <row r="18" spans="1:14">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" t="s">
+        <v>55</v>
+      </c>
+      <c r="J18" t="s">
+        <v>38</v>
+      </c>
+      <c r="K18" t="s">
+        <v>56</v>
+      </c>
+      <c r="L18" t="s">
+        <v>44</v>
+      </c>
+      <c r="M18" t="s">
+        <v>44</v>
+      </c>
+      <c r="N18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" t="s">
+        <v>83</v>
+      </c>
+      <c r="J19" t="s">
+        <v>84</v>
+      </c>
+      <c r="K19" t="s">
+        <v>85</v>
+      </c>
+      <c r="L19" t="s">
+        <v>44</v>
+      </c>
+      <c r="M19" t="s">
+        <v>44</v>
+      </c>
+      <c r="N19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" t="s">
+        <v>56</v>
+      </c>
+      <c r="L20" t="s">
+        <v>44</v>
+      </c>
+      <c r="M20" t="s">
+        <v>44</v>
+      </c>
+      <c r="N20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" t="s">
+        <v>38</v>
+      </c>
+      <c r="K21" t="s">
+        <v>56</v>
+      </c>
+      <c r="L21" t="s">
+        <v>44</v>
+      </c>
+      <c r="M21" t="s">
+        <v>44</v>
+      </c>
+      <c r="N21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" t="s">
+        <v>67</v>
+      </c>
+      <c r="J22" t="s">
+        <v>68</v>
+      </c>
+      <c r="K22" t="s">
+        <v>69</v>
+      </c>
+      <c r="L22" t="s">
+        <v>44</v>
+      </c>
+      <c r="M22" t="s">
+        <v>44</v>
+      </c>
+      <c r="N22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" t="s">
+        <v>44</v>
+      </c>
+      <c r="M23" t="s">
+        <v>44</v>
+      </c>
+      <c r="N23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" t="s">
+        <v>44</v>
+      </c>
+      <c r="M24" t="s">
+        <v>44</v>
+      </c>
+      <c r="N24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" t="s">
+        <v>27</v>
+      </c>
+      <c r="J25" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" t="s">
+        <v>44</v>
+      </c>
+      <c r="M25" t="s">
+        <v>44</v>
+      </c>
+      <c r="N25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" t="s">
+        <v>27</v>
+      </c>
+      <c r="J26" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" t="s">
+        <v>22</v>
+      </c>
+      <c r="L26" t="s">
+        <v>44</v>
+      </c>
+      <c r="M26" t="s">
+        <v>44</v>
+      </c>
+      <c r="N26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" t="s">
+        <v>28</v>
+      </c>
+      <c r="H27" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27" t="s">
+        <v>27</v>
+      </c>
+      <c r="J27" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" t="s">
+        <v>44</v>
+      </c>
+      <c r="M27" t="s">
+        <v>44</v>
+      </c>
+      <c r="N27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" t="s">
+        <v>27</v>
+      </c>
+      <c r="J28" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" t="s">
+        <v>44</v>
+      </c>
+      <c r="M28" t="s">
+        <v>44</v>
+      </c>
+      <c r="N28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" t="s">
+        <v>22</v>
+      </c>
+      <c r="L29" t="s">
+        <v>44</v>
+      </c>
+      <c r="M29" t="s">
+        <v>44</v>
+      </c>
+      <c r="N29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" t="s">
+        <v>27</v>
+      </c>
+      <c r="G30" t="s">
+        <v>28</v>
+      </c>
+      <c r="H30" t="s">
+        <v>21</v>
+      </c>
+      <c r="I30" t="s">
+        <v>27</v>
+      </c>
+      <c r="J30" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" t="s">
+        <v>22</v>
+      </c>
+      <c r="L30" t="s">
+        <v>44</v>
+      </c>
+      <c r="M30" t="s">
+        <v>44</v>
+      </c>
+      <c r="N30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" t="s">
+        <v>27</v>
+      </c>
+      <c r="J31" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" t="s">
+        <v>22</v>
+      </c>
+      <c r="L31" t="s">
+        <v>44</v>
+      </c>
+      <c r="M31" t="s">
+        <v>44</v>
+      </c>
+      <c r="N31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" t="s">
+        <v>28</v>
+      </c>
+      <c r="H32" t="s">
+        <v>21</v>
+      </c>
+      <c r="I32" t="s">
+        <v>27</v>
+      </c>
+      <c r="J32" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32" t="s">
+        <v>22</v>
+      </c>
+      <c r="L32" t="s">
+        <v>44</v>
+      </c>
+      <c r="M32" t="s">
+        <v>44</v>
+      </c>
+      <c r="N32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H33" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33" t="s">
+        <v>27</v>
+      </c>
+      <c r="J33" t="s">
+        <v>21</v>
+      </c>
+      <c r="K33" t="s">
+        <v>22</v>
+      </c>
+      <c r="L33" t="s">
+        <v>44</v>
+      </c>
+      <c r="M33" t="s">
+        <v>44</v>
+      </c>
+      <c r="N33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" t="s">
+        <v>27</v>
+      </c>
+      <c r="G34" t="s">
+        <v>28</v>
+      </c>
+      <c r="H34" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" t="s">
+        <v>27</v>
+      </c>
+      <c r="J34" t="s">
+        <v>21</v>
+      </c>
+      <c r="K34" t="s">
+        <v>22</v>
+      </c>
+      <c r="L34" t="s">
+        <v>44</v>
+      </c>
+      <c r="M34" t="s">
+        <v>44</v>
+      </c>
+      <c r="N34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" t="s">
+        <v>27</v>
+      </c>
+      <c r="G35" t="s">
+        <v>28</v>
+      </c>
+      <c r="H35" t="s">
+        <v>21</v>
+      </c>
+      <c r="I35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J35" t="s">
+        <v>21</v>
+      </c>
+      <c r="K35" t="s">
+        <v>22</v>
+      </c>
+      <c r="L35" t="s">
+        <v>44</v>
+      </c>
+      <c r="M35" t="s">
+        <v>44</v>
+      </c>
+      <c r="N35" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
fix import library issues
</commit_message>
<xml_diff>
--- a/TestSuite-API/reports/daily_reading_report.xlsx
+++ b/TestSuite-API/reports/daily_reading_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="107">
   <si>
     <t>Date
 Period</t>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>17-10-27 ~ 17-10-28</t>
+  </si>
+  <si>
+    <t>17-10-28 ~ 17-10-29</t>
   </si>
 </sst>
 </file>
@@ -724,7 +727,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
       <selection activeCell="A25" sqref="A25"/>
@@ -2233,6 +2236,50 @@
         <v>32</v>
       </c>
     </row>
+    <row r="36" spans="1:14">
+      <c r="A36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" t="s">
+        <v>28</v>
+      </c>
+      <c r="H36" t="s">
+        <v>21</v>
+      </c>
+      <c r="I36" t="s">
+        <v>34</v>
+      </c>
+      <c r="J36" t="s">
+        <v>21</v>
+      </c>
+      <c r="K36" t="s">
+        <v>22</v>
+      </c>
+      <c r="L36" t="s">
+        <v>44</v>
+      </c>
+      <c r="M36" t="s">
+        <v>44</v>
+      </c>
+      <c r="N36" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
fixed name error of test case
</commit_message>
<xml_diff>
--- a/TestSuite-API/reports/daily_reading_report.xlsx
+++ b/TestSuite-API/reports/daily_reading_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
   <si>
     <t>Date
 Period</t>
@@ -346,6 +346,15 @@
   </si>
   <si>
     <t>17-10-28 ~ 17-10-29</t>
+  </si>
+  <si>
+    <t>17-10-31 ~ 17-11-01</t>
+  </si>
+  <si>
+    <t>6.25%</t>
+  </si>
+  <si>
+    <t>['7ff9010202000024', '7ff9010202000025', '7ff9010202000026', '7ff9010202000027', '7ff9010202000028']</t>
   </si>
 </sst>
 </file>
@@ -727,7 +736,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
       <selection activeCell="A25" sqref="A25"/>
@@ -2280,6 +2289,50 @@
         <v>46</v>
       </c>
     </row>
+    <row r="37" spans="1:14">
+      <c r="A37" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37" t="s">
+        <v>55</v>
+      </c>
+      <c r="G37" t="s">
+        <v>28</v>
+      </c>
+      <c r="H37" t="s">
+        <v>55</v>
+      </c>
+      <c r="I37" t="s">
+        <v>21</v>
+      </c>
+      <c r="J37" t="s">
+        <v>21</v>
+      </c>
+      <c r="K37" t="s">
+        <v>22</v>
+      </c>
+      <c r="L37" t="s">
+        <v>44</v>
+      </c>
+      <c r="M37" t="s">
+        <v>109</v>
+      </c>
+      <c r="N37" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>